<commit_message>
Egresos manejo de la funcion guardar
</commit_message>
<xml_diff>
--- a/assets/plantillas/egresos.xlsx
+++ b/assets/plantillas/egresos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aplicaciones web\Programas con pyton\proyectoC\assets\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125B57E6-C78B-4DBF-9604-2FA488C9E62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF908132-ED68-4E1A-AC8B-851138F55373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>PÓLIZA DE EGRESO</t>
   </si>
@@ -88,24 +88,6 @@
   </si>
   <si>
     <t>C. JOSÉ EDUARDO MARTÍNEZ CRUZ</t>
-  </si>
-  <si>
-    <t>21/05/2025</t>
-  </si>
-  <si>
-    <t>Sadriel</t>
-  </si>
-  <si>
-    <t>EFECTIVO</t>
-  </si>
-  <si>
-    <t>iludyiegsrliq09876</t>
-  </si>
-  <si>
-    <t>xd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ni una </t>
   </si>
 </sst>
 </file>
@@ -1087,13 +1069,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>13220</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>54</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>13220</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1110,8 +1092,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="4330148"/>
-          <a:ext cx="9565171" cy="4969565"/>
+          <a:off x="0" y="4240794"/>
+          <a:ext cx="9471881" cy="4920363"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3365,8 +3347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="101" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="BK35" sqref="BK35"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="BN10" sqref="BN10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.15"/>
@@ -4416,9 +4398,7 @@
       <c r="AU5" s="11"/>
       <c r="AV5" s="11"/>
       <c r="AW5" s="38"/>
-      <c r="AX5" s="57" t="s">
-        <v>19</v>
-      </c>
+      <c r="AX5" s="57"/>
       <c r="AY5" s="57"/>
       <c r="AZ5" s="57"/>
       <c r="BA5" s="57"/>
@@ -4523,9 +4503,7 @@
       <c r="AN8" s="43"/>
       <c r="AO8" s="43"/>
       <c r="AP8" s="43"/>
-      <c r="AQ8" s="44">
-        <v>45798</v>
-      </c>
+      <c r="AQ8" s="44"/>
       <c r="AR8" s="45"/>
       <c r="AS8" s="45"/>
       <c r="AT8" s="45"/>
@@ -4540,9 +4518,7 @@
       <c r="BC8" s="45"/>
     </row>
     <row r="9" spans="1:64" s="1" customFormat="1" ht="25.55" customHeight="1">
-      <c r="A9" s="46" t="s">
-        <v>20</v>
-      </c>
+      <c r="A9" s="46"/>
       <c r="B9" s="46"/>
       <c r="C9" s="46"/>
       <c r="D9" s="46"/>
@@ -4582,9 +4558,7 @@
       <c r="AL9" s="46"/>
       <c r="AM9" s="46"/>
       <c r="AN9" s="46"/>
-      <c r="AO9" s="47">
-        <v>10</v>
-      </c>
+      <c r="AO9" s="47"/>
       <c r="AP9" s="48"/>
       <c r="AQ9" s="48"/>
       <c r="AR9" s="48"/>
@@ -4683,9 +4657,7 @@
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="T12" s="51" t="s">
-        <v>21</v>
-      </c>
+      <c r="T12" s="51"/>
       <c r="U12" s="51"/>
       <c r="V12" s="51"/>
       <c r="W12" s="51"/>
@@ -4718,9 +4690,7 @@
       <c r="BC12" s="39"/>
     </row>
     <row r="13" spans="1:64" s="1" customFormat="1" ht="25.55" customHeight="1">
-      <c r="A13" s="64" t="s">
-        <v>22</v>
-      </c>
+      <c r="A13" s="64"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
@@ -7043,9 +7013,7 @@
       <c r="BK43" s="28"/>
     </row>
     <row r="44" spans="1:256" s="25" customFormat="1" ht="30.7" customHeight="1">
-      <c r="A44" s="89" t="s">
-        <v>23</v>
-      </c>
+      <c r="A44" s="89"/>
       <c r="B44" s="90"/>
       <c r="C44" s="90"/>
       <c r="D44" s="90"/>
@@ -7377,9 +7345,7 @@
       <c r="IV46" s="88"/>
     </row>
     <row r="47" spans="1:256">
-      <c r="A47" s="105" t="s">
-        <v>24</v>
-      </c>
+      <c r="A47" s="105"/>
       <c r="B47" s="95"/>
       <c r="C47" s="95"/>
       <c r="D47" s="95"/>

</xml_diff>